<commit_message>
Add more tests; clean more code
</commit_message>
<xml_diff>
--- a/input/tests/TEST_lvl2-instructions.xlsx
+++ b/input/tests/TEST_lvl2-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>iso</t>
   </si>
@@ -63,12 +63,6 @@
     <t>deu</t>
   </si>
   <si>
-    <t>agg_fuel</t>
-  </si>
-  <si>
-    <t>coal</t>
-  </si>
-  <si>
     <t>match_to_trend</t>
   </si>
   <si>
@@ -79,6 +73,9 @@
   </si>
   <si>
     <t>end_continuity</t>
+  </si>
+  <si>
+    <t>coal coke</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -463,7 +460,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -473,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -485,13 +482,13 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -499,7 +496,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1937</v>

</xml_diff>

<commit_message>
Bug fixes and code refactoring
</commit_message>
<xml_diff>
--- a/input/tests/TEST_lvl2-instructions.xlsx
+++ b/input/tests/TEST_lvl2-instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16335" windowHeight="17445" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16335" windowHeight="17445" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interpolation_instructions" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>end_continuity</t>
   </si>
   <si>
-    <t>coal coke</t>
+    <t>hard_coal</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>